<commit_message>
aggregate next5 Oi and Di
</commit_message>
<xml_diff>
--- a/FootballPoisson.xlsx
+++ b/FootballPoisson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvtm2\Desktop\Python\FootballPoisson\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intern\Desktop\FootballPoisson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4757AB3-3355-4F9C-A63F-D1492EA95761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB6072D-3738-4388-822C-8AA24627AD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Data" sheetId="1" r:id="rId1"/>
@@ -130,25 +130,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="3"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -156,7 +149,7 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -164,7 +157,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -172,15 +165,19 @@
     <font>
       <b/>
       <sz val="16"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="16"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,22 +200,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -503,11 +501,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -516,11 +514,11 @@
     <col min="5" max="5" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="9.140625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="15" width="9.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -546,7 +544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -568,15 +566,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="8">
-        <f t="shared" ref="G2:G22" si="2">E2/$B$24</f>
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="H2" s="8">
-        <f t="shared" ref="H2:H22" si="3">F2/$B$24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -597,16 +593,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G3" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -628,15 +622,13 @@
         <v>1</v>
       </c>
       <c r="G4" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="3"/>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -657,16 +649,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G5" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -688,15 +678,13 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -717,16 +705,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G7" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -747,16 +733,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -778,15 +762,13 @@
         <v>3</v>
       </c>
       <c r="G9" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="3"/>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -808,15 +790,13 @@
         <v>1</v>
       </c>
       <c r="G10" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="3"/>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -838,15 +818,13 @@
         <v>2</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="3"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -867,16 +845,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G12" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -898,15 +874,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" si="2"/>
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
@@ -927,16 +901,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G14" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
@@ -958,15 +930,13 @@
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
@@ -988,15 +958,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
@@ -1018,15 +986,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -1048,15 +1014,13 @@
         <v>1</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="3"/>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
@@ -1077,16 +1041,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
@@ -1107,16 +1069,14 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1138,15 +1098,13 @@
         <v>2</v>
       </c>
       <c r="G21" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" si="3"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
@@ -1171,15 +1129,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G22" s="8" t="e">
-        <f t="shared" si="2"/>
+        <f>E22/$B$24</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H22" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <f>F22/$B$24</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -1189,7 +1147,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1199,19 +1156,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="9" width="9.140625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1227,168 +1184,287 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="9"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="11">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
+      <c r="G21" s="11">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated README and coloring in fixtures sheet
</commit_message>
<xml_diff>
--- a/FootballPoisson.xlsx
+++ b/FootballPoisson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yutsz/Desktop/FootballPoisson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intern\Desktop\FootballPoisson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A76FC19-6E2A-4047-8560-07788B9B117D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1824445B-2DAE-4C9A-BC42-27C228E8B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1820" windowWidth="25000" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="450" windowWidth="28080" windowHeight="16830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Data" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,8 +303,39 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +354,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -347,34 +402,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,651 +735,673 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="9.1640625" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="3"/>
+    <col min="9" max="18" width="9.140625" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="19">
         <v>4</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="19">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8">
-        <v>2</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="D2" s="19">
+        <v>2</v>
+      </c>
+      <c r="E2" s="20">
+        <v>2</v>
+      </c>
+      <c r="F2" s="20">
         <v>0</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="21">
         <v>1.51</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="19">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="D3" s="19">
+        <v>2</v>
+      </c>
+      <c r="E3" s="20">
+        <v>1</v>
+      </c>
+      <c r="F3" s="20">
         <v>1.5</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="21">
         <v>0.75</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="21">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9">
+      <c r="B4" s="19">
+        <v>2</v>
+      </c>
+      <c r="C4" s="19">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19">
+        <v>2</v>
+      </c>
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
         <v>0.75</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="21">
         <v>0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B5" s="19">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
         <v>3</v>
       </c>
-      <c r="D5" s="7">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20">
         <v>1.5</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="21">
         <v>0.75</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="21">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="19">
         <v>5</v>
       </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2</v>
+      </c>
+      <c r="E6" s="20">
         <v>2.5</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="20">
         <v>0.5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="21">
         <v>1.89</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="21">
         <v>0.38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="19">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="19">
         <v>4</v>
       </c>
-      <c r="D7" s="7">
-        <v>2</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="D7" s="19">
+        <v>2</v>
+      </c>
+      <c r="E7" s="20">
         <v>3</v>
       </c>
-      <c r="F7" s="8">
-        <v>2</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="F7" s="20">
+        <v>2</v>
+      </c>
+      <c r="G7" s="21">
         <v>2.2599999999999998</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="21">
         <v>1.51</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" s="19">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19">
         <v>4</v>
       </c>
-      <c r="D8" s="7">
-        <v>2</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="D8" s="19">
+        <v>2</v>
+      </c>
+      <c r="E8" s="20">
         <v>0.5</v>
       </c>
-      <c r="F8" s="8">
-        <v>2</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="F8" s="20">
+        <v>2</v>
+      </c>
+      <c r="G8" s="21">
         <v>0.38</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="21">
         <v>1.51</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="19">
         <v>0</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="19">
         <v>7</v>
       </c>
-      <c r="D9" s="7">
-        <v>2</v>
-      </c>
-      <c r="E9" s="8">
+      <c r="D9" s="19">
+        <v>2</v>
+      </c>
+      <c r="E9" s="20">
         <v>0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="20">
         <v>3.5</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="21">
         <v>0</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="21">
         <v>2.64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7">
-        <v>2</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="B10" s="19">
+        <v>2</v>
+      </c>
+      <c r="C10" s="19">
+        <v>2</v>
+      </c>
+      <c r="D10" s="19">
+        <v>2</v>
+      </c>
+      <c r="E10" s="20">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21">
         <v>0.75</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="21">
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="19">
+        <v>1</v>
+      </c>
+      <c r="C11" s="19">
         <v>6</v>
       </c>
-      <c r="D11" s="7">
-        <v>2</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="D11" s="19">
+        <v>2</v>
+      </c>
+      <c r="E11" s="20">
         <v>0.5</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="20">
         <v>3</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="21">
         <v>0.38</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="21">
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7">
-        <v>2</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="19">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
-        <v>2</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="D12" s="19">
+        <v>2</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20">
         <v>1.5</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="21">
         <v>0.75</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="21">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="19">
         <v>4</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="19">
         <v>0</v>
       </c>
-      <c r="D13" s="7">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="D13" s="19">
+        <v>2</v>
+      </c>
+      <c r="E13" s="20">
+        <v>2</v>
+      </c>
+      <c r="F13" s="20">
         <v>0</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="21">
         <v>1.51</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="19">
         <v>6</v>
       </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>2</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19">
+        <v>2</v>
+      </c>
+      <c r="E14" s="20">
         <v>3</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="20">
         <v>0.5</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="21">
         <v>2.2599999999999998</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="21">
         <v>0.38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="7">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7">
-        <v>2</v>
-      </c>
-      <c r="E15" s="8">
-        <v>1</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="B15" s="19">
+        <v>2</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2</v>
+      </c>
+      <c r="D15" s="19">
+        <v>2</v>
+      </c>
+      <c r="E15" s="20">
+        <v>1</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1</v>
+      </c>
+      <c r="G15" s="21">
         <v>0.75</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="21">
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="7">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>2</v>
-      </c>
-      <c r="E16" s="8">
-        <v>1</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="B16" s="19">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19">
+        <v>2</v>
+      </c>
+      <c r="E16" s="20">
+        <v>1</v>
+      </c>
+      <c r="F16" s="20">
         <v>0.5</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="21">
         <v>0.75</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="21">
         <v>0.38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="7">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7">
-        <v>2</v>
-      </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="B17" s="19">
+        <v>2</v>
+      </c>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>2</v>
+      </c>
+      <c r="E17" s="20">
+        <v>1</v>
+      </c>
+      <c r="F17" s="20">
         <v>0.5</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="21">
         <v>0.75</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="21">
         <v>0.38</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="19">
         <v>0</v>
       </c>
-      <c r="C18" s="7">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7">
-        <v>2</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="C18" s="19">
+        <v>2</v>
+      </c>
+      <c r="D18" s="19">
+        <v>2</v>
+      </c>
+      <c r="E18" s="20">
         <v>0</v>
       </c>
-      <c r="F18" s="8">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9">
+      <c r="F18" s="20">
+        <v>1</v>
+      </c>
+      <c r="G18" s="21">
         <v>0</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="21">
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="19">
         <v>5</v>
       </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
-        <v>2</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="C19" s="19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="20">
         <v>2.5</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="20">
         <v>0.5</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="21">
         <v>1.89</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="21">
         <v>0.38</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="19">
         <v>3</v>
       </c>
-      <c r="C20" s="7">
-        <v>2</v>
-      </c>
-      <c r="D20" s="7">
-        <v>2</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C20" s="19">
+        <v>2</v>
+      </c>
+      <c r="D20" s="19">
+        <v>2</v>
+      </c>
+      <c r="E20" s="20">
         <v>1.5</v>
       </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9">
+      <c r="F20" s="20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="21">
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="7">
-        <v>2</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B21" s="19">
+        <v>2</v>
+      </c>
+      <c r="C21" s="19">
         <v>8</v>
       </c>
-      <c r="D21" s="7">
-        <v>2</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="D21" s="19">
+        <v>2</v>
+      </c>
+      <c r="E21" s="20">
+        <v>1</v>
+      </c>
+      <c r="F21" s="20">
         <v>4</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="21">
         <v>0.75</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="21">
         <v>3.02</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="22">
         <v>53</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="22">
         <v>53</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="22">
         <v>40</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="20">
         <v>1.325</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="20">
         <v>1.325</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="21">
         <v>0.99799999999999989</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="21">
         <v>0.99899999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="21">
         <v>1.325</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1312,568 +1412,568 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.1640625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="3"/>
+    <col min="1" max="1" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="9.140625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="1">
-        <v>13.58</v>
-      </c>
-      <c r="H2" s="1">
-        <v>6.04</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="G2" s="8">
+        <v>6.7899999999999991</v>
+      </c>
+      <c r="H2" s="8">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="1">
-        <v>5.26</v>
-      </c>
-      <c r="H3" s="1">
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="G3" s="10">
+        <v>2.63</v>
+      </c>
+      <c r="H3" s="11">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="1">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="H4" s="1">
-        <v>12.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="G4" s="5">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H4" s="11">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="1">
-        <v>12.06</v>
-      </c>
-      <c r="H5" s="1">
-        <v>10.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="G5" s="8">
+        <v>6.0299999999999994</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5.2799999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="1">
-        <v>13.58</v>
-      </c>
-      <c r="H6" s="1">
-        <v>9.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="G6" s="8">
+        <v>6.79</v>
+      </c>
+      <c r="H6" s="5">
+        <v>4.5299999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="1">
-        <v>9.7999999999999989</v>
-      </c>
-      <c r="H7" s="1">
-        <v>7.54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="G7" s="5">
+        <v>4.8999999999999986</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="1">
-        <v>10.54</v>
-      </c>
-      <c r="H8" s="1">
-        <v>12.06</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="G8" s="5">
+        <v>5.27</v>
+      </c>
+      <c r="H8" s="5">
+        <v>6.0299999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1">
-        <v>6.76</v>
-      </c>
-      <c r="H9" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="G9" s="10">
+        <v>3.38</v>
+      </c>
+      <c r="H9" s="5">
+        <v>4.8999999999999986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="1">
-        <v>10.54</v>
-      </c>
-      <c r="H10" s="1">
-        <v>8.2999999999999989</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="G10" s="5">
+        <v>5.27</v>
+      </c>
+      <c r="H10" s="5">
+        <v>4.1499999999999986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="1">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="H11" s="1">
-        <v>7.52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="G11" s="5">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="1">
-        <v>6.78</v>
-      </c>
-      <c r="H12" s="1">
-        <v>12.06</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="G12" s="10">
+        <v>3.39</v>
+      </c>
+      <c r="H12" s="5">
+        <v>6.0299999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="1">
-        <v>6.76</v>
-      </c>
-      <c r="H13" s="1">
-        <v>12.82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="G13" s="10">
+        <v>3.38</v>
+      </c>
+      <c r="H13" s="11">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="1">
-        <v>9.7799999999999994</v>
-      </c>
-      <c r="H14" s="1">
-        <v>6.02</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="G14" s="5">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="H14" s="8">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="1">
-        <v>9.06</v>
-      </c>
-      <c r="H15" s="1">
-        <v>7.5399999999999991</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="G15" s="5">
+        <v>4.53</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="1">
-        <v>11.3</v>
-      </c>
-      <c r="H16" s="1">
-        <v>14.34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="G16" s="5">
+        <v>5.6499999999999986</v>
+      </c>
+      <c r="H16" s="11">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="1">
-        <v>14.32</v>
-      </c>
-      <c r="H17" s="1">
-        <v>11.32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="G17" s="8">
+        <v>7.1599999999999993</v>
+      </c>
+      <c r="H17" s="5">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="1">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="H18" s="1">
-        <v>9.7799999999999994</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="G18" s="10">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="H18" s="5">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="1">
-        <v>11.3</v>
-      </c>
-      <c r="H19" s="1">
-        <v>5.28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="G19" s="5">
+        <v>5.6499999999999986</v>
+      </c>
+      <c r="H19" s="8">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="1">
-        <v>12.8</v>
-      </c>
-      <c r="H20" s="1">
-        <v>12.06</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="G20" s="8">
+        <v>6.3999999999999986</v>
+      </c>
+      <c r="H20" s="11">
+        <v>6.0299999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="1">
-        <v>9.02</v>
-      </c>
-      <c r="H21" s="1">
-        <v>6.04</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="5">
+        <v>4.51</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1883,18 +1983,23 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G23" s="1">
-        <v>9.98</v>
-      </c>
-      <c r="H23" s="1">
-        <v>9.9899999999999984</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="5">
+        <v>4.99</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4.9949999999999992</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>78</v>
       </c>
@@ -1905,37 +2010,41 @@
         <v>10</v>
       </c>
       <c r="D24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+    </row>
+    <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="25" t="s">
         <v>24</v>
       </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>